<commit_message>
Windows vs Linux url issues
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10405"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\eclipse-jee-mars-2-win32-x86_64\eclipse\DIGINode\surveillancetest\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kesavarajumudunuri/Desktop/1800/LiveViewTechQAAuto/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EAA201-F7D4-524A-AFB9-AF0285704013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="3"/>
+    <workbookView xWindow="540" yWindow="460" windowWidth="19420" windowHeight="10420" tabRatio="863" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Logintest" sheetId="22" r:id="rId1"/>
@@ -22,18 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="80">
   <si>
     <t>TestID</t>
   </si>
@@ -270,12 +265,15 @@
   </si>
   <si>
     <t>Deactive</t>
+  </si>
+  <si>
+    <t>vkalyan.babu@contractor.liveviewtech.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -682,26 +680,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,7 +714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -723,40 +722,44 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
+        <v>65</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{C71B437C-72AE-5748-9E28-4FE53671BA4D}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{8F8D6BDF-D762-9348-80C7-29FD756356D1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -773,7 +776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -781,42 +784,46 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>65</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{17F6EED5-6959-7E4E-B085-42FACD691F21}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{BC15154A-FBFE-C34F-AA27-ADE3F91016E8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
@@ -825,7 +832,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -857,7 +864,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -865,10 +872,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>35</v>
@@ -878,7 +885,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -886,10 +893,10 @@
         <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>21</v>
@@ -904,7 +911,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -912,10 +919,10 @@
         <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
@@ -932,7 +939,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -940,10 +947,10 @@
         <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>29</v>
@@ -958,7 +965,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -966,10 +973,10 @@
         <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>30</v>
@@ -986,7 +993,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -994,10 +1001,10 @@
         <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>32</v>
@@ -1014,7 +1021,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1022,10 +1029,10 @@
         <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>33</v>
@@ -1034,7 +1041,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
@@ -1042,10 +1049,10 @@
         <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>34</v>
@@ -1055,7 +1062,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -1063,10 +1070,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
@@ -1075,7 +1082,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
@@ -1083,10 +1090,10 @@
         <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
@@ -1095,7 +1102,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
@@ -1103,10 +1110,10 @@
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E13" t="s">
         <v>38</v>
@@ -1115,7 +1122,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -1123,10 +1130,10 @@
         <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>35</v>
@@ -1135,7 +1142,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -1143,10 +1150,10 @@
         <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E15" t="s">
         <v>39</v>
@@ -1155,7 +1162,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>53</v>
       </c>
@@ -1163,10 +1170,10 @@
         <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>40</v>
@@ -1175,7 +1182,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
@@ -1183,10 +1190,10 @@
         <v>23</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>14</v>
+        <v>79</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E17" t="s">
         <v>41</v>
@@ -1195,7 +1202,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>45</v>
       </c>
@@ -1208,7 +1215,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +1244,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -1267,31 +1274,37 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{8A520866-B58D-F04D-9C2C-F0F46FD69975}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{316F94AA-6108-8740-977A-5B8722A77327}"/>
+    <hyperlink ref="D4:D17" r:id="rId3" display="Kb100684@" xr:uid="{C34D5F06-08F3-2A48-A3DA-5F309DAE2B27}"/>
+    <hyperlink ref="C4:C17" r:id="rId4" display="vkalyan.babu@contractor.liveviewtech.com" xr:uid="{CF9A6583-9C05-3C4D-91F8-3385365C10B1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>70</v>
       </c>
@@ -1299,7 +1312,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1332,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1339,12 +1352,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1377,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1384,12 +1397,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E12" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1411,9 +1424,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C13" r:id="rId2"/>
-    <hyperlink ref="C8" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C13" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{7EB295F3-76A3-DD44-9258-B5819B1D0546}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding The email properties
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="114">
   <si>
     <t>TestID</t>
   </si>
@@ -315,9 +315,6 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Default Landing Page</t>
-  </si>
-  <si>
     <t>NotificationProtocol</t>
   </si>
   <si>
@@ -334,6 +331,51 @@
   </si>
   <si>
     <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>DefaultLandingPage</t>
+  </si>
+  <si>
+    <t>Password@123</t>
+  </si>
+  <si>
+    <t>LVTTest</t>
+  </si>
+  <si>
+    <t>Legacy Player</t>
+  </si>
+  <si>
+    <t>LVT Customer Service</t>
+  </si>
+  <si>
+    <t>Blue Eye</t>
+  </si>
+  <si>
+    <t>//test</t>
+  </si>
+  <si>
+    <t>AddNewuser</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>kesav.m+kalyans@contractor.liveviewtech.com</t>
+  </si>
+  <si>
+    <t>@gileKalyan123</t>
+  </si>
+  <si>
+    <t>UserPassword</t>
+  </si>
+  <si>
+    <t>LiveView Technologies</t>
+  </si>
+  <si>
+    <t>LVTTestAutomation</t>
   </si>
 </sst>
 </file>
@@ -865,7 +907,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F2" sqref="F2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,14 +1536,19 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1512,85 +1559,147 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>98</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>97</v>
       </c>
       <c r="K2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>95</v>
       </c>
       <c r="Q2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="W2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="X2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y2" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="X2" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE2" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>66</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" t="s">
+        <v>103</v>
+      </c>
+      <c r="W3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B4" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId1" display="LVTTestAutomation@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the code for generic Actions and test cases.
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Logintest" sheetId="22" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="D3CommandCenterTest" sheetId="24" r:id="rId3"/>
     <sheet name="LiveUnits" sheetId="25" r:id="rId4"/>
     <sheet name="AddNewUser" sheetId="26" r:id="rId5"/>
+    <sheet name="Notifications" sheetId="27" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="121">
   <si>
     <t>TestID</t>
   </si>
@@ -376,6 +377,27 @@
   </si>
   <si>
     <t>LVTTestAutomation</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>aarbuckle@archnexus.com</t>
+  </si>
+  <si>
+    <t>Aaron Arbuckle</t>
+  </si>
+  <si>
+    <t>Okland Construction</t>
+  </si>
+  <si>
+    <t>1203@keanegrp.com</t>
+  </si>
+  <si>
+    <t>aatkinson@jacobsenconstruction.com</t>
   </si>
 </sst>
 </file>
@@ -1527,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AE4" sqref="AE4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,4 +1724,105 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4" display="https://qa.liveviewtech.com/users/view/5821"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the code for Client Create
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\eclipse-jee-mars-2-win32-x86_64\eclipse\DIGINode\surveillancetest\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\Survelince\surveillancetest\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="5"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Logintest" sheetId="22" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="LiveUnits" sheetId="25" r:id="rId4"/>
     <sheet name="AddNewUser" sheetId="26" r:id="rId5"/>
     <sheet name="Notifications" sheetId="27" r:id="rId6"/>
+    <sheet name="CreateNewClient" sheetId="28" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="209">
   <si>
     <t>TestID</t>
   </si>
@@ -398,13 +399,277 @@
   </si>
   <si>
     <t>aatkinson@jacobsenconstruction.com</t>
+  </si>
+  <si>
+    <t>CreateNewClient</t>
+  </si>
+  <si>
+    <t>AccountRep</t>
+  </si>
+  <si>
+    <t>Timeout</t>
+  </si>
+  <si>
+    <t>LiveViewtes1</t>
+  </si>
+  <si>
+    <t>AUS ACT</t>
+  </si>
+  <si>
+    <t>IOS Dev</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>CreateNewClientWithAllFields</t>
+  </si>
+  <si>
+    <t>EmailDomain</t>
+  </si>
+  <si>
+    <t>ParentClient</t>
+  </si>
+  <si>
+    <t>BillableClient</t>
+  </si>
+  <si>
+    <t>SalesRep</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>SLA</t>
+  </si>
+  <si>
+    <t>SalesContact</t>
+  </si>
+  <si>
+    <t>SalesPhone</t>
+  </si>
+  <si>
+    <t>SalesMobile</t>
+  </si>
+  <si>
+    <t>SalesEmail</t>
+  </si>
+  <si>
+    <t>BillingContact</t>
+  </si>
+  <si>
+    <t>BillingPhone</t>
+  </si>
+  <si>
+    <t>BillingMobile</t>
+  </si>
+  <si>
+    <t>BillingEmail</t>
+  </si>
+  <si>
+    <t>TechnicalEmail</t>
+  </si>
+  <si>
+    <t>TechnicalContact</t>
+  </si>
+  <si>
+    <t>TechnicalPhone</t>
+  </si>
+  <si>
+    <t>TechnicalMobile</t>
+  </si>
+  <si>
+    <t>SecurityKey</t>
+  </si>
+  <si>
+    <t>MapCenterLatitude</t>
+  </si>
+  <si>
+    <t>MapCenterLongitude</t>
+  </si>
+  <si>
+    <t>MapZoomLevel</t>
+  </si>
+  <si>
+    <t>MapType</t>
+  </si>
+  <si>
+    <t>CameraNavigationMode</t>
+  </si>
+  <si>
+    <t>DefaultView</t>
+  </si>
+  <si>
+    <t>LogoImageName</t>
+  </si>
+  <si>
+    <t>VideoOverlayImage</t>
+  </si>
+  <si>
+    <t>AuthenticationEmailLinkDomain</t>
+  </si>
+  <si>
+    <t>ClientDomainRedirect</t>
+  </si>
+  <si>
+    <t>PublicVideoTimeout</t>
+  </si>
+  <si>
+    <t>PublicViewMode</t>
+  </si>
+  <si>
+    <t>OldFTPServer</t>
+  </si>
+  <si>
+    <t>WatermarkTextforImages</t>
+  </si>
+  <si>
+    <t>WelcomeEmailMessage</t>
+  </si>
+  <si>
+    <t>thisClientsUsers</t>
+  </si>
+  <si>
+    <t>OtherClientsUsers</t>
+  </si>
+  <si>
+    <t>StreamingServer</t>
+  </si>
+  <si>
+    <t>PatrolServer</t>
+  </si>
+  <si>
+    <t>DataExpiration</t>
+  </si>
+  <si>
+    <t>TermsOfServiceText</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>useD3CommandCenter</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>hyd</t>
+  </si>
+  <si>
+    <t>ind</t>
+  </si>
+  <si>
+    <t>mub</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>789</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Celsius</t>
+  </si>
+  <si>
+    <t>Liveview</t>
+  </si>
+  <si>
+    <t>AEDG</t>
+  </si>
+  <si>
+    <t>LVTA</t>
+  </si>
+  <si>
+    <t>www.lvt.com</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>abcde@gmail.com</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>Road Map</t>
+  </si>
+  <si>
+    <t>Plain Camera List</t>
+  </si>
+  <si>
+    <t>Camera Map</t>
+  </si>
+  <si>
+    <t>lvt</t>
+  </si>
+  <si>
+    <t>lvt1</t>
+  </si>
+  <si>
+    <t>http://abc@gmail.com</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Live Video</t>
+  </si>
+  <si>
+    <t>abcdefdg</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>hi live</t>
+  </si>
+  <si>
+    <t>Security Operator and Above</t>
+  </si>
+  <si>
+    <t>Client Admins and Above</t>
+  </si>
+  <si>
+    <t>UDOT</t>
+  </si>
+  <si>
+    <t>USW2A</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>hhhhh</t>
+  </si>
+  <si>
+    <t>klyn</t>
+  </si>
+  <si>
+    <t>on</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +696,12 @@
       <color rgb="FF333333"/>
       <name val="Lucida Sans Unicode"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -472,7 +743,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -491,6 +762,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1730,7 +2004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1825,4 +2099,858 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CA7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="2"/>
+      <c r="BM1" s="2"/>
+      <c r="BN1" s="2"/>
+      <c r="BO1" s="2"/>
+      <c r="BP1" s="2"/>
+      <c r="BQ1" s="2"/>
+      <c r="BR1" s="2"/>
+      <c r="BS1" s="2"/>
+      <c r="BT1" s="2"/>
+      <c r="BU1" s="2"/>
+      <c r="BV1" s="2"/>
+      <c r="BW1" s="2"/>
+      <c r="BX1" s="2"/>
+      <c r="BY1" s="2"/>
+      <c r="BZ1" s="2"/>
+      <c r="CA1" s="2"/>
+    </row>
+    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+      <c r="BD2" s="2"/>
+      <c r="BE2" s="2"/>
+      <c r="BF2" s="2"/>
+      <c r="BG2" s="2"/>
+      <c r="BH2" s="2"/>
+      <c r="BI2" s="2"/>
+      <c r="BJ2" s="2"/>
+      <c r="BK2" s="2"/>
+      <c r="BL2" s="2"/>
+      <c r="BM2" s="2"/>
+      <c r="BN2" s="2"/>
+      <c r="BO2" s="2"/>
+      <c r="BP2" s="2"/>
+      <c r="BQ2" s="2"/>
+      <c r="BR2" s="2"/>
+      <c r="BS2" s="2"/>
+      <c r="BT2" s="2"/>
+      <c r="BU2" s="2"/>
+      <c r="BV2" s="2"/>
+      <c r="BW2" s="2"/>
+      <c r="BX2" s="2"/>
+      <c r="BY2" s="2"/>
+      <c r="BZ2" s="2"/>
+      <c r="CA2" s="2"/>
+    </row>
+    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2"/>
+      <c r="BE3" s="2"/>
+      <c r="BF3" s="2"/>
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2"/>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2"/>
+      <c r="BK3" s="2"/>
+      <c r="BL3" s="2"/>
+      <c r="BM3" s="2"/>
+      <c r="BN3" s="2"/>
+      <c r="BO3" s="2"/>
+      <c r="BP3" s="2"/>
+      <c r="BQ3" s="2"/>
+      <c r="BR3" s="2"/>
+      <c r="BS3" s="2"/>
+      <c r="BT3" s="2"/>
+      <c r="BU3" s="2"/>
+      <c r="BV3" s="2"/>
+      <c r="BW3" s="2"/>
+      <c r="BX3" s="2"/>
+      <c r="BY3" s="2"/>
+      <c r="BZ3" s="2"/>
+      <c r="CA3" s="2"/>
+    </row>
+    <row r="4" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="2"/>
+      <c r="BD4" s="2"/>
+      <c r="BE4" s="2"/>
+      <c r="BF4" s="2"/>
+      <c r="BG4" s="2"/>
+      <c r="BH4" s="2"/>
+      <c r="BI4" s="2"/>
+      <c r="BJ4" s="2"/>
+      <c r="BK4" s="2"/>
+      <c r="BL4" s="2"/>
+      <c r="BM4" s="2"/>
+      <c r="BN4" s="2"/>
+      <c r="BO4" s="2"/>
+      <c r="BP4" s="2"/>
+      <c r="BQ4" s="2"/>
+      <c r="BR4" s="2"/>
+      <c r="BS4" s="2"/>
+      <c r="BT4" s="2"/>
+      <c r="BU4" s="2"/>
+      <c r="BV4" s="2"/>
+      <c r="BW4" s="2"/>
+      <c r="BX4" s="2"/>
+      <c r="BY4" s="2"/>
+      <c r="BZ4" s="2"/>
+      <c r="CA4" s="2"/>
+    </row>
+    <row r="5" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="2"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="2"/>
+      <c r="BD5" s="2"/>
+      <c r="BE5" s="2"/>
+      <c r="BF5" s="2"/>
+      <c r="BG5" s="2"/>
+      <c r="BH5" s="2"/>
+      <c r="BI5" s="2"/>
+      <c r="BJ5" s="2"/>
+      <c r="BK5" s="2"/>
+      <c r="BL5" s="2"/>
+      <c r="BM5" s="2"/>
+      <c r="BN5" s="2"/>
+      <c r="BO5" s="2"/>
+      <c r="BP5" s="2"/>
+      <c r="BQ5" s="2"/>
+      <c r="BR5" s="2"/>
+      <c r="BS5" s="2"/>
+      <c r="BT5" s="2"/>
+      <c r="BU5" s="2"/>
+      <c r="BV5" s="2"/>
+      <c r="BW5" s="2"/>
+      <c r="BX5" s="2"/>
+      <c r="BY5" s="2"/>
+      <c r="BZ5" s="2"/>
+      <c r="CA5" s="2"/>
+    </row>
+    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG6" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="AH6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AJ6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK6" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AM6" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AN6" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AO6" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP6" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AS6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AT6" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AU6" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="AV6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW6" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="AX6" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="AY6" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="AZ6" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="BA6" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="BB6" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="BC6" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="BD6" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="BE6" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="BF6" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="BG6" s="7"/>
+      <c r="BH6" s="7"/>
+      <c r="BI6" s="7"/>
+      <c r="BJ6" s="7"/>
+      <c r="BK6" s="7"/>
+      <c r="BL6" s="7"/>
+      <c r="BM6" s="7"/>
+      <c r="BN6" s="7"/>
+      <c r="BO6" s="7"/>
+      <c r="BP6" s="7"/>
+      <c r="BQ6" s="7"/>
+      <c r="BR6" s="7"/>
+      <c r="BS6" s="7"/>
+      <c r="BT6" s="7"/>
+      <c r="BU6" s="7"/>
+      <c r="BV6" s="7"/>
+      <c r="BW6" s="7"/>
+      <c r="BX6" s="7"/>
+      <c r="BY6" s="7"/>
+      <c r="BZ6" s="7"/>
+      <c r="CA6" s="7"/>
+    </row>
+    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y7" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC7" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD7" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE7" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AF7" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="AG7" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="AH7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI7" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="AJ7" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="AK7" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL7" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="AM7" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="AN7" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AO7" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="AP7" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="AQ7" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="AR7" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="AS7" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT7" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU7" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="AV7" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW7" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="AX7" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AY7" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AZ7" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="BA7" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="BB7" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="BC7" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="BD7" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="BE7" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="BF7" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="BG7" s="2"/>
+      <c r="BH7" s="2"/>
+      <c r="BI7" s="2"/>
+      <c r="BJ7" s="2"/>
+      <c r="BK7" s="2"/>
+      <c r="BL7" s="2"/>
+      <c r="BM7" s="2"/>
+      <c r="BN7" s="2"/>
+      <c r="BO7" s="2"/>
+      <c r="BP7" s="2"/>
+      <c r="BQ7" s="2"/>
+      <c r="BR7" s="2"/>
+      <c r="BS7" s="2"/>
+      <c r="BT7" s="2"/>
+      <c r="BU7" s="2"/>
+      <c r="BV7" s="2"/>
+      <c r="BW7" s="2"/>
+      <c r="BX7" s="2"/>
+      <c r="BY7" s="2"/>
+      <c r="BZ7" s="2"/>
+      <c r="CA7" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="H7" r:id="rId3"/>
+    <hyperlink ref="S7" r:id="rId4"/>
+    <hyperlink ref="Y7" r:id="rId5"/>
+    <hyperlink ref="AC7" r:id="rId6"/>
+    <hyperlink ref="AQ7" r:id="rId7"/>
+    <hyperlink ref="AD7" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add new user with All fields
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="6"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863"/>
   </bookViews>
   <sheets>
     <sheet name="Logintest" sheetId="22" r:id="rId1"/>
@@ -1087,15 +1087,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,13 +1125,16 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
+        <v>65</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2105,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding the new Role and Updated the date code for Reports
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Logintest" sheetId="22" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="214">
   <si>
     <t>TestID</t>
   </si>
@@ -75,12 +75,6 @@
   </si>
   <si>
     <t>LoginTest1</t>
-  </si>
-  <si>
-    <t>scott.abbott@liveviewtech.com</t>
-  </si>
-  <si>
-    <t>Royalfire1</t>
   </si>
   <si>
     <t>RevenuePerLiveUnitTest</t>
@@ -1109,14 +1103,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,15 +1141,15 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1165,7 +1160,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1174,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1196,7 +1191,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1207,18 +1202,21 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1226,15 +1224,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
@@ -1244,7 +1243,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1265,22 +1264,22 @@
         <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1288,20 +1287,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H3" s="6"/>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1309,25 +1308,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1335,27 +1334,27 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1363,25 +1362,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1389,27 +1388,27 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1417,213 +1416,213 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1648,19 +1647,19 @@
         <v>11</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1668,33 +1667,51 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>14</v>
+        <v>107</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="C10" r:id="rId8"/>
+    <hyperlink ref="C11" r:id="rId9"/>
+    <hyperlink ref="C12" r:id="rId10"/>
+    <hyperlink ref="C13" r:id="rId11"/>
+    <hyperlink ref="C14" r:id="rId12"/>
+    <hyperlink ref="C15" r:id="rId13"/>
+    <hyperlink ref="C16" r:id="rId14"/>
+    <hyperlink ref="C17" r:id="rId15"/>
+    <hyperlink ref="C24" r:id="rId16"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -1702,7 +1719,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1717,7 +1736,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1734,13 +1753,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1748,24 +1767,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1779,13 +1798,13 @@
         <v>11</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>74</v>
-      </c>
       <c r="F7" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1793,16 +1812,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -1810,7 +1829,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1818,26 +1837,26 @@
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" t="s">
         <v>73</v>
       </c>
-      <c r="E13" t="s">
-        <v>75</v>
-      </c>
       <c r="F13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C13" r:id="rId2"/>
-    <hyperlink ref="C8" r:id="rId3"/>
+    <hyperlink ref="C13" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1847,8 +1866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,7 +1885,7 @@
   <sheetData>
     <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -1880,88 +1899,88 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="N2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="V2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="W2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>93</v>
-      </c>
       <c r="Z2" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AA2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="AD2" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -1969,90 +1988,90 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="G3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="N3" s="14">
         <v>90001</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="R3" s="14" t="s">
+      <c r="U3" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="S3" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="U3" s="14" t="s">
-        <v>215</v>
-      </c>
       <c r="V3" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AC3" s="2"/>
       <c r="AD3" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -2103,7 +2122,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2117,7 +2136,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2133,16 +2152,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2150,41 +2169,41 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2192,7 +2211,7 @@
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="D9" r:id="rId2"/>
     <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4" display="https://qa.liveviewtech.com/users/view/5821"/>
+    <hyperlink ref="D3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
@@ -2204,14 +2223,17 @@
   <dimension ref="A1:CA7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2303,16 +2325,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2392,22 +2414,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>127</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2565,7 +2587,7 @@
     </row>
     <row r="5" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2657,169 +2679,169 @@
         <v>11</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG6" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="AH6" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="AJ6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AK6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AM6" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AN6" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO6" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP6" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="AR6" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS6" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z6" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA6" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB6" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC6" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE6" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="AF6" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="AG6" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="AH6" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="AI6" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="AJ6" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="AK6" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AL6" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="AM6" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="AN6" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="AO6" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="AP6" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="AQ6" s="7" t="s">
+      <c r="AT6" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="AR6" s="7" t="s">
+      <c r="AU6" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="AS6" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="AT6" s="7" t="s">
+      <c r="AV6" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="AU6" s="7" t="s">
+      <c r="AW6" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="AV6" s="7" t="s">
+      <c r="AX6" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="AW6" s="7" t="s">
+      <c r="AY6" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="AX6" s="7" t="s">
+      <c r="AZ6" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="AY6" s="7" t="s">
+      <c r="BA6" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="AZ6" s="7" t="s">
+      <c r="BB6" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="BA6" s="7" t="s">
+      <c r="BC6" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="BB6" s="7" t="s">
+      <c r="BD6" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="BC6" s="7" t="s">
+      <c r="BE6" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="BD6" s="7" t="s">
+      <c r="BF6" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="BE6" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="BF6" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="BG6" s="7"/>
       <c r="BH6" s="7"/>
@@ -2848,173 +2870,173 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>127</v>
-      </c>
       <c r="H7" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="M7" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="O7" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="S7" s="11" t="s">
         <v>180</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="S7" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="V7" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="X7" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="W7" s="12" t="s">
+      <c r="Y7" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="X7" s="12" t="s">
+      <c r="Z7" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AC7" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="Y7" s="11" t="s">
+      <c r="AD7" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="AE7" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF7" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="AG7" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AH7" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI7" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="Z7" s="12" t="s">
+      <c r="AJ7" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="AK7" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="AA7" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB7" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC7" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="AD7" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="AE7" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="AF7" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="AG7" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="AH7" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI7" s="10" t="s">
+      <c r="AL7" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="AJ7" s="12" t="s">
+      <c r="AM7" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="AK7" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="AL7" s="13" t="s">
+      <c r="AN7" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="AM7" s="13" t="s">
+      <c r="AO7" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="AN7" s="13" t="s">
+      <c r="AP7" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="AO7" s="13" t="s">
+      <c r="AQ7" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="AP7" s="13" t="s">
+      <c r="AR7" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="AQ7" s="11" t="s">
+      <c r="AS7" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AT7" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="AU7" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="AR7" s="13" t="s">
+      <c r="AV7" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="AS7" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="AT7" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU7" s="13" t="s">
+      <c r="AW7" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="AV7" s="2" t="s">
+      <c r="AX7" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="AW7" s="12" t="s">
+      <c r="AY7" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="AX7" s="2" t="s">
+      <c r="AZ7" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="AY7" s="13" t="s">
+      <c r="BA7" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="AZ7" s="13" t="s">
+      <c r="BB7" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="BA7" s="2" t="s">
+      <c r="BC7" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="BB7" s="13" t="s">
+      <c r="BD7" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="BC7" s="14" t="s">
+      <c r="BE7" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="BD7" s="2" t="s">
+      <c r="BF7" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="BE7" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="BF7" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="BG7" s="2"/>
       <c r="BH7" s="2"/>

</xml_diff>

<commit_message>
UPdated the code with new Data.
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -19,6 +19,7 @@
     <sheet name="AddNewUser" sheetId="26" r:id="rId5"/>
     <sheet name="Notifications" sheetId="27" r:id="rId6"/>
     <sheet name="CreateNewClient" sheetId="28" r:id="rId7"/>
+    <sheet name="AddNewRoleTest" sheetId="29" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="222">
   <si>
     <t>TestID</t>
   </si>
@@ -143,9 +144,6 @@
     <t>LVT Accounting</t>
   </si>
   <si>
-    <t>LVT Customer service" user</t>
-  </si>
-  <si>
     <t>LVT Infrastructure</t>
   </si>
   <si>
@@ -155,15 +153,9 @@
     <t>Camera Operator (Presets, PTZF)</t>
   </si>
   <si>
-    <t>Client administrator with Analytics</t>
-  </si>
-  <si>
     <t>RunMode</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -678,6 +670,39 @@
   </si>
   <si>
     <t>26</t>
+  </si>
+  <si>
+    <t>AddNewRole</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TestRole</t>
+  </si>
+  <si>
+    <t>Test description</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Aaron Auer</t>
+  </si>
+  <si>
+    <t>aauer@nd.gov</t>
+  </si>
+  <si>
+    <t>1TestClient</t>
+  </si>
+  <si>
+    <t>Client Administrator with Analytics</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>UserEmaiIid</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1128,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,10 +1166,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1160,7 +1185,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,10 +1227,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
@@ -1222,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,7 +1266,7 @@
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -1250,7 +1275,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1264,25 +1289,34 @@
         <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1290,20 +1324,29 @@
         <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="J3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="6"/>
+      <c r="L3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1311,25 +1354,34 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1337,27 +1389,35 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1365,25 +1425,34 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1391,27 +1460,34 @@
         <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1419,210 +1495,297 @@
         <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="6" t="s">
+      <c r="J8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="J10" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M17" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1633,7 +1796,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>0</v>
       </c>
@@ -1647,10 +1810,10 @@
         <v>11</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>17</v>
@@ -1659,27 +1822,27 @@
         <v>24</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G24" t="s">
         <v>29</v>
@@ -1688,30 +1851,17 @@
         <v>29</v>
       </c>
       <c r="I24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
-    <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
-    <hyperlink ref="C7" r:id="rId5"/>
-    <hyperlink ref="C8" r:id="rId6"/>
-    <hyperlink ref="C9" r:id="rId7"/>
-    <hyperlink ref="C10" r:id="rId8"/>
-    <hyperlink ref="C11" r:id="rId9"/>
-    <hyperlink ref="C12" r:id="rId10"/>
-    <hyperlink ref="C13" r:id="rId11"/>
-    <hyperlink ref="C14" r:id="rId12"/>
-    <hyperlink ref="C15" r:id="rId13"/>
-    <hyperlink ref="C16" r:id="rId14"/>
-    <hyperlink ref="C17" r:id="rId15"/>
-    <hyperlink ref="C24" r:id="rId16"/>
+    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="M3" r:id="rId2" display="https://qa.liveviewtech.com/clients/view/1050/2"/>
+    <hyperlink ref="M12" r:id="rId3" display="https://qa.liveviewtech.com/clients/view/1050/2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1736,7 +1886,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1753,13 +1903,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1767,24 +1917,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1798,13 +1948,13 @@
         <v>11</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1812,16 +1962,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -1829,7 +1979,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1837,19 +1987,19 @@
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
         <v>73</v>
-      </c>
-      <c r="F13" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1885,7 +2035,7 @@
   <sheetData>
     <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -1899,70 +2049,70 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="J2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="K2" s="8" t="s">
+      <c r="O2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="L2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="U2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>17</v>
@@ -1977,10 +2127,10 @@
         <v>25</v>
       </c>
       <c r="AD2" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -1988,73 +2138,73 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="G3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="N3" s="14">
         <v>90001</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="U3" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="R3" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="S3" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="U3" s="14" t="s">
-        <v>213</v>
-      </c>
       <c r="V3" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>10</v>
@@ -2064,14 +2214,14 @@
       </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="AC3" s="2"/>
       <c r="AD3" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -2136,7 +2286,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2152,16 +2302,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2169,19 +2319,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
@@ -2189,13 +2339,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>32</v>
@@ -2203,7 +2353,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2223,7 +2373,7 @@
   <dimension ref="A1:CA7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +2383,7 @@
   <sheetData>
     <row r="1" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2325,16 +2475,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2414,22 +2564,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>122</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>125</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2587,7 +2737,7 @@
     </row>
     <row r="5" spans="1:79" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2679,169 +2829,169 @@
         <v>11</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H6" s="7" t="s">
+      <c r="L6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="R6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="P6" s="7" t="s">
+      <c r="S6" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="T6" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="U6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="V6" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="W6" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="T6" s="7" t="s">
+      <c r="X6" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="U6" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="V6" s="7" t="s">
+      <c r="Y6" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="W6" s="7" t="s">
+      <c r="Z6" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="X6" s="7" t="s">
+      <c r="AA6" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="Y6" s="7" t="s">
+      <c r="AB6" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="Z6" s="7" t="s">
+      <c r="AC6" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="AA6" s="7" t="s">
+      <c r="AD6" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="AB6" s="7" t="s">
+      <c r="AE6" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AC6" s="7" t="s">
+      <c r="AF6" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="AD6" s="7" t="s">
+      <c r="AG6" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="AE6" s="7" t="s">
+      <c r="AH6" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="AF6" s="7" t="s">
+      <c r="AI6" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="AG6" s="7" t="s">
+      <c r="AJ6" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="AH6" s="7" t="s">
+      <c r="AK6" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="AI6" s="7" t="s">
+      <c r="AL6" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AJ6" s="7" t="s">
+      <c r="AM6" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="AK6" s="7" t="s">
+      <c r="AN6" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AL6" s="7" t="s">
+      <c r="AO6" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="AM6" s="7" t="s">
+      <c r="AP6" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="AN6" s="7" t="s">
+      <c r="AQ6" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="AO6" s="7" t="s">
+      <c r="AR6" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="AP6" s="7" t="s">
+      <c r="AS6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT6" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="AQ6" s="7" t="s">
+      <c r="AU6" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="AR6" s="7" t="s">
+      <c r="AV6" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AS6" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="AT6" s="7" t="s">
+      <c r="AW6" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="AU6" s="7" t="s">
+      <c r="AX6" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="AV6" s="7" t="s">
+      <c r="AY6" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="AW6" s="7" t="s">
+      <c r="AZ6" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="AX6" s="7" t="s">
+      <c r="BA6" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="AY6" s="7" t="s">
+      <c r="BB6" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="AZ6" s="7" t="s">
+      <c r="BC6" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="BA6" s="7" t="s">
+      <c r="BD6" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="BB6" s="7" t="s">
+      <c r="BE6" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="BC6" s="7" t="s">
+      <c r="BF6" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="BD6" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="BE6" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="BF6" s="7" t="s">
-        <v>168</v>
       </c>
       <c r="BG6" s="7"/>
       <c r="BH6" s="7"/>
@@ -2870,173 +3020,173 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>125</v>
-      </c>
       <c r="H7" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="M7" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="P7" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="S7" s="11" t="s">
         <v>177</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="S7" s="11" t="s">
-        <v>180</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="V7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y7" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="W7" s="12" t="s">
+      <c r="Z7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="AC7" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="X7" s="12" t="s">
+      <c r="AD7" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="AE7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF7" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="AG7" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="AH7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI7" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="Y7" s="11" t="s">
+      <c r="AJ7" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="Z7" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA7" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="AB7" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="AC7" s="11" t="s">
+      <c r="AK7" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="AL7" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="AD7" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="AE7" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="AF7" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG7" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="AH7" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI7" s="10" t="s">
+      <c r="AM7" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="AJ7" s="12" t="s">
+      <c r="AN7" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="AK7" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="AL7" s="13" t="s">
+      <c r="AO7" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="AM7" s="13" t="s">
+      <c r="AP7" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="AN7" s="13" t="s">
+      <c r="AQ7" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="AO7" s="13" t="s">
+      <c r="AR7" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="AP7" s="13" t="s">
+      <c r="AS7" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT7" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="AU7" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="AQ7" s="11" t="s">
+      <c r="AV7" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="AR7" s="13" t="s">
+      <c r="AW7" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="AS7" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT7" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="AU7" s="13" t="s">
+      <c r="AX7" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="AV7" s="2" t="s">
+      <c r="AY7" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="AW7" s="12" t="s">
+      <c r="AZ7" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="AX7" s="2" t="s">
+      <c r="BA7" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="AY7" s="13" t="s">
+      <c r="BB7" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="AZ7" s="13" t="s">
+      <c r="BC7" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="BA7" s="2" t="s">
+      <c r="BD7" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="BB7" s="13" t="s">
+      <c r="BE7" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="BC7" s="14" t="s">
+      <c r="BF7" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="BD7" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="BE7" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="BF7" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="BG7" s="2"/>
       <c r="BH7" s="2"/>
@@ -3073,4 +3223,70 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the new Changes
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\Survelince\surveillancetest\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\LiveViewTech\Agile367\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="10430" tabRatio="863" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Logintest" sheetId="22" r:id="rId1"/>
@@ -20,6 +20,10 @@
     <sheet name="Notifications" sheetId="27" r:id="rId6"/>
     <sheet name="CreateNewClient" sheetId="28" r:id="rId7"/>
     <sheet name="AddNewRoleTest" sheetId="29" r:id="rId8"/>
+    <sheet name="ModemPageTest" sheetId="30" r:id="rId9"/>
+    <sheet name="ViewProfilePageTest" sheetId="31" r:id="rId10"/>
+    <sheet name="HomePageTest" sheetId="33" r:id="rId11"/>
+    <sheet name="BoxPageTest" sheetId="32" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="335">
   <si>
     <t>TestID</t>
   </si>
@@ -231,9 +235,6 @@
     <t>SelectDate</t>
   </si>
   <si>
-    <t>2/14/2020</t>
-  </si>
-  <si>
     <t>ArchiveLiveUnits</t>
   </si>
   <si>
@@ -703,13 +704,355 @@
   </si>
   <si>
     <t>UserEmaiIid</t>
+  </si>
+  <si>
+    <t>8/07/2020</t>
+  </si>
+  <si>
+    <t>ModemPage</t>
+  </si>
+  <si>
+    <t>ModemMftrs</t>
+  </si>
+  <si>
+    <t>MEID</t>
+  </si>
+  <si>
+    <t>SIM1</t>
+  </si>
+  <si>
+    <t>SIM2</t>
+  </si>
+  <si>
+    <t>WANMACAddress</t>
+  </si>
+  <si>
+    <t>WLANMACAddress</t>
+  </si>
+  <si>
+    <t>FirmwareVersion</t>
+  </si>
+  <si>
+    <t>OwnedbyClient</t>
+  </si>
+  <si>
+    <t>CalculatedIPAddress</t>
+  </si>
+  <si>
+    <t>VPNIPAddress</t>
+  </si>
+  <si>
+    <t>DVNIPAddress</t>
+  </si>
+  <si>
+    <t>LANIPAddress</t>
+  </si>
+  <si>
+    <t>LANSubnetMask</t>
+  </si>
+  <si>
+    <t>LANGateway</t>
+  </si>
+  <si>
+    <t>VpnServers</t>
+  </si>
+  <si>
+    <t>WANIPAddress</t>
+  </si>
+  <si>
+    <t>WANSubnetMask</t>
+  </si>
+  <si>
+    <t>WANGateway</t>
+  </si>
+  <si>
+    <t>WANDNS1</t>
+  </si>
+  <si>
+    <t>WANDNS2</t>
+  </si>
+  <si>
+    <t>WANDNS3</t>
+  </si>
+  <si>
+    <t>WANPort</t>
+  </si>
+  <si>
+    <t>UsesHTTPS</t>
+  </si>
+  <si>
+    <t>RelayNumber</t>
+  </si>
+  <si>
+    <t>WirelessSSID</t>
+  </si>
+  <si>
+    <t>WirelessChannel</t>
+  </si>
+  <si>
+    <t>WirelessEncryptionID</t>
+  </si>
+  <si>
+    <t>WirelessPassword</t>
+  </si>
+  <si>
+    <t>AdministrationUserName</t>
+  </si>
+  <si>
+    <t>AdministrationPassword</t>
+  </si>
+  <si>
+    <t>ISP</t>
+  </si>
+  <si>
+    <t>ISPAccountNumber</t>
+  </si>
+  <si>
+    <t>IsISPAccountOwnedbyClient</t>
+  </si>
+  <si>
+    <t>PurchaseOrderNumber</t>
+  </si>
+  <si>
+    <t>FullnameofpersonwholasttestedModem</t>
+  </si>
+  <si>
+    <t>UsageHistoryofModem</t>
+  </si>
+  <si>
+    <t>MultipleModemMftrs</t>
+  </si>
+  <si>
+    <t>SerialNumbers</t>
+  </si>
+  <si>
+    <t>MultiplePurchaseOrderNumber</t>
+  </si>
+  <si>
+    <t>MultipleNotes</t>
+  </si>
+  <si>
+    <t>Modem1</t>
+  </si>
+  <si>
+    <t>DPC3825</t>
+  </si>
+  <si>
+    <t>94414</t>
+  </si>
+  <si>
+    <t>94415</t>
+  </si>
+  <si>
+    <t>123467</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>VZWPrimary</t>
+  </si>
+  <si>
+    <t>567</t>
+  </si>
+  <si>
+    <t>gateway1</t>
+  </si>
+  <si>
+    <t>WAN1</t>
+  </si>
+  <si>
+    <t>WAN2</t>
+  </si>
+  <si>
+    <t>WAN3</t>
+  </si>
+  <si>
+    <t>Port1</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>4567</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>pswd</t>
+  </si>
+  <si>
+    <t>ATT</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>notes1</t>
+  </si>
+  <si>
+    <t>PX-500</t>
+  </si>
+  <si>
+    <t>Note1</t>
+  </si>
+  <si>
+    <t>ViewProfilePageTest</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>MobilePhone</t>
+  </si>
+  <si>
+    <t>PushNotificationsEnabled</t>
+  </si>
+  <si>
+    <t>LoginExpiration</t>
+  </si>
+  <si>
+    <t>AllowedtouseD3CommandCenter</t>
+  </si>
+  <si>
+    <t>SecurityDashboardQueue</t>
+  </si>
+  <si>
+    <t>RequirePasswordChange</t>
+  </si>
+  <si>
+    <t>SignedClientTOS</t>
+  </si>
+  <si>
+    <t>LoginCount</t>
+  </si>
+  <si>
+    <t>LastLogin</t>
+  </si>
+  <si>
+    <t>ToursViewed</t>
+  </si>
+  <si>
+    <t>DateCreated</t>
+  </si>
+  <si>
+    <t>DateModified</t>
+  </si>
+  <si>
+    <t>CreatedBy</t>
+  </si>
+  <si>
+    <t>ModifiedBy</t>
+  </si>
+  <si>
+    <t>kalyan.babu@contractor.liveviewtech.com (SAML)</t>
+  </si>
+  <si>
+    <t>Kalyan</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>street11</t>
+  </si>
+  <si>
+    <t>IQ1</t>
+  </si>
+  <si>
+    <t>city1</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Mountain Time</t>
+  </si>
+  <si>
+    <t>1231231234</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>{No Expiration}</t>
+  </si>
+  <si>
+    <t>Low Latency (inherited)</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>389</t>
+  </si>
+  <si>
+    <t>2020-06-22 2:13:59am</t>
+  </si>
+  <si>
+    <t>2020-04-06 6:06:23am</t>
+  </si>
+  <si>
+    <t>2020-06-18 12:02:13pm</t>
+  </si>
+  <si>
+    <t>Kesav (userID: 9385)</t>
+  </si>
+  <si>
+    <t>Kalyan (userID: 9389)</t>
+  </si>
+  <si>
+    <t>Boxpage</t>
+  </si>
+  <si>
+    <t>BoxVersion</t>
+  </si>
+  <si>
+    <t>RevisionNumber</t>
+  </si>
+  <si>
+    <t>DocumentationURL</t>
+  </si>
+  <si>
+    <t>Boxes</t>
+  </si>
+  <si>
+    <t>Newbox1</t>
+  </si>
+  <si>
+    <t>www.LiveView.Com</t>
+  </si>
+  <si>
+    <t>HomePageTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,8 +1086,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Lucida Sans Unicode"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -769,8 +1118,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -778,12 +1133,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -805,6 +1169,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1128,23 +1504,23 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1158,7 +1534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1166,15 +1542,417 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="27.36328125" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="AE3" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="26.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="32.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="G3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1188,21 +1966,21 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1227,10 +2005,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
@@ -1249,24 +2027,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38:N39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -1275,7 +2053,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1289,10 +2067,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>221</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
@@ -1313,10 +2091,10 @@
         <v>38</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1324,16 +2102,16 @@
         <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E3" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>33</v>
@@ -1343,10 +2121,10 @@
         <v>39</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1354,16 +2132,16 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E4" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>19</v>
@@ -1378,10 +2156,10 @@
         <v>39</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1389,16 +2167,16 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E5" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>20</v>
@@ -1414,10 +2192,10 @@
         <v>39</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1425,16 +2203,16 @@
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E6" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
@@ -1449,10 +2227,10 @@
         <v>39</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1460,16 +2238,16 @@
         <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E7" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>28</v>
@@ -1484,10 +2262,10 @@
         <v>39</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1495,16 +2273,16 @@
         <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E8" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>30</v>
@@ -1519,10 +2297,10 @@
         <v>39</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -1530,16 +2308,16 @@
         <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E9" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>31</v>
@@ -1548,10 +2326,10 @@
         <v>39</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -1559,16 +2337,16 @@
         <v>21</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E10" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>32</v>
@@ -1577,10 +2355,10 @@
         <v>39</v>
       </c>
       <c r="M10" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -1588,16 +2366,16 @@
         <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E11" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>34</v>
@@ -1606,10 +2384,10 @@
         <v>39</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1617,28 +2395,28 @@
         <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E12" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>217</v>
-      </c>
       <c r="G12" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
@@ -1646,16 +2424,16 @@
         <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E13" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>35</v>
@@ -1664,10 +2442,10 @@
         <v>39</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
@@ -1675,16 +2453,16 @@
         <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E14" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>33</v>
@@ -1693,10 +2471,10 @@
         <v>39</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>47</v>
       </c>
@@ -1704,16 +2482,16 @@
         <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E15" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>36</v>
@@ -1722,10 +2500,10 @@
         <v>39</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
@@ -1733,16 +2511,16 @@
         <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E16" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>37</v>
@@ -1751,10 +2529,10 @@
         <v>39</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -1762,28 +2540,28 @@
         <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="E17" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>217</v>
-      </c>
       <c r="G17" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>39</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -1796,7 +2574,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>0</v>
       </c>
@@ -1825,7 +2603,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -1833,10 +2611,10 @@
         <v>50</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>56</v>
@@ -1870,29 +2648,29 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1912,15 +2690,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="D3" t="s">
         <v>62</v>
@@ -1929,15 +2707,15 @@
         <v>59</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
@@ -1948,41 +2726,41 @@
         <v>11</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="D8" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E12" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1993,13 +2771,13 @@
         <v>61</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2020,25 +2798,25 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="2"/>
+    <col min="11" max="11" width="21.1796875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2049,70 +2827,70 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="X2" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="W2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>17</v>
@@ -2127,84 +2905,84 @@
         <v>25</v>
       </c>
       <c r="AD2" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE2" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AE2" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="D3" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="N3" s="14">
         <v>90001</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="R3" s="14" t="s">
+      <c r="S3" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="S3" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="U3" s="14" t="s">
-        <v>210</v>
-      </c>
       <c r="V3" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>10</v>
@@ -2214,17 +2992,17 @@
       </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AC3" s="2"/>
       <c r="AD3" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="11"/>
       <c r="C4" s="2"/>
@@ -2275,23 +3053,23 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2302,58 +3080,58 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="D3" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
         <v>112</v>
-      </c>
-      <c r="F3" t="s">
-        <v>113</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D5" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D9" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2376,14 +3154,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2464,7 +3242,7 @@
       <c r="BZ1" s="2"/>
       <c r="CA1" s="2"/>
     </row>
-    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2475,16 +3253,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2559,27 +3337,27 @@
       <c r="BZ2" s="2"/>
       <c r="CA2" s="2"/>
     </row>
-    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="D3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="10" t="s">
         <v>121</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>122</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2654,7 +3432,7 @@
       <c r="BZ3" s="2"/>
       <c r="CA3" s="2"/>
     </row>
-    <row r="4" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2735,9 +3513,9 @@
       <c r="BZ4" s="2"/>
       <c r="CA4" s="2"/>
     </row>
-    <row r="5" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2818,7 +3596,7 @@
       <c r="BZ5" s="2"/>
       <c r="CA5" s="2"/>
     </row>
-    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -2829,169 +3607,169 @@
         <v>11</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="H6" s="7" t="s">
+      <c r="K6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="P6" s="7" t="s">
+      <c r="Q6" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="R6" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="S6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="T6" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="T6" s="7" t="s">
+      <c r="U6" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="V6" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="U6" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="V6" s="7" t="s">
+      <c r="W6" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="W6" s="7" t="s">
+      <c r="X6" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="X6" s="7" t="s">
+      <c r="Y6" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="Y6" s="7" t="s">
+      <c r="Z6" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="Z6" s="7" t="s">
+      <c r="AA6" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="AA6" s="7" t="s">
+      <c r="AB6" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="AB6" s="7" t="s">
+      <c r="AC6" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="AC6" s="7" t="s">
+      <c r="AD6" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="AD6" s="7" t="s">
+      <c r="AE6" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="AE6" s="7" t="s">
+      <c r="AF6" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AF6" s="7" t="s">
+      <c r="AG6" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="AG6" s="7" t="s">
+      <c r="AH6" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="AH6" s="7" t="s">
+      <c r="AI6" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="AI6" s="7" t="s">
+      <c r="AJ6" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="AJ6" s="7" t="s">
+      <c r="AK6" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="AK6" s="7" t="s">
+      <c r="AL6" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="AL6" s="7" t="s">
+      <c r="AM6" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AM6" s="7" t="s">
+      <c r="AN6" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="AN6" s="7" t="s">
+      <c r="AO6" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AO6" s="7" t="s">
+      <c r="AP6" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="AP6" s="7" t="s">
+      <c r="AQ6" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="AQ6" s="7" t="s">
+      <c r="AR6" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="AR6" s="7" t="s">
+      <c r="AS6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT6" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="AS6" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="AT6" s="7" t="s">
+      <c r="AU6" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="AU6" s="7" t="s">
+      <c r="AV6" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="AV6" s="7" t="s">
+      <c r="AW6" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AW6" s="7" t="s">
+      <c r="AX6" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="AX6" s="7" t="s">
+      <c r="AY6" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="AY6" s="7" t="s">
+      <c r="AZ6" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="AZ6" s="7" t="s">
+      <c r="BA6" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="BA6" s="7" t="s">
+      <c r="BB6" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="BB6" s="7" t="s">
+      <c r="BC6" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="BC6" s="7" t="s">
+      <c r="BD6" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="BD6" s="7" t="s">
+      <c r="BE6" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="BE6" s="7" t="s">
+      <c r="BF6" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="BF6" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="BG6" s="7"/>
       <c r="BH6" s="7"/>
@@ -3015,178 +3793,178 @@
       <c r="BZ6" s="7"/>
       <c r="CA6" s="7"/>
     </row>
-    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="D7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>122</v>
-      </c>
       <c r="H7" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="N7" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="S7" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="V7" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="W7" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="W7" s="12" t="s">
+      <c r="X7" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="X7" s="12" t="s">
+      <c r="Y7" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="Y7" s="11" t="s">
+      <c r="Z7" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="AC7" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="Z7" s="12" t="s">
+      <c r="AD7" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE7" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF7" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="AA7" s="12" t="s">
+      <c r="AG7" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="AB7" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="AC7" s="11" t="s">
+      <c r="AH7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI7" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="AD7" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="AE7" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="AF7" s="12" t="s">
+      <c r="AJ7" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AK7" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="AG7" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH7" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI7" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="AJ7" s="12" t="s">
+      <c r="AL7" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="AK7" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="AL7" s="13" t="s">
+      <c r="AM7" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="AM7" s="13" t="s">
+      <c r="AN7" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="AN7" s="13" t="s">
+      <c r="AO7" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="AO7" s="13" t="s">
+      <c r="AP7" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="AP7" s="13" t="s">
+      <c r="AQ7" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="AQ7" s="11" t="s">
+      <c r="AR7" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="AR7" s="13" t="s">
+      <c r="AS7" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT7" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="AU7" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="AS7" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="AT7" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="AU7" s="13" t="s">
+      <c r="AV7" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="AV7" s="2" t="s">
+      <c r="AW7" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="AW7" s="12" t="s">
+      <c r="AX7" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="AX7" s="2" t="s">
+      <c r="AY7" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="AY7" s="13" t="s">
+      <c r="AZ7" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="AZ7" s="13" t="s">
+      <c r="BA7" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="BA7" s="2" t="s">
+      <c r="BB7" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="BB7" s="13" t="s">
+      <c r="BC7" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="BC7" s="14" t="s">
+      <c r="BD7" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="BD7" s="2" t="s">
+      <c r="BE7" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="BE7" s="2" t="s">
+      <c r="BF7" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="BF7" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="BG7" s="2"/>
       <c r="BH7" s="2"/>
@@ -3229,23 +4007,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -3256,37 +4034,393 @@
         <v>11</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
         <v>104</v>
       </c>
-      <c r="C3" t="s">
-        <v>105</v>
-      </c>
       <c r="D3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" t="s">
         <v>213</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>214</v>
-      </c>
-      <c r="F3" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AU3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="AM2" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="AN2" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="AO2" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="AP2" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="AQ2" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="AR2" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="AS2" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="AT2" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="AU2" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="U3" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC3" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD3" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="AE3" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="AF3" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="AJ3" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="AK3" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL3" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="AR3" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="AT3" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Updating the tets cases"
This reverts commit 50eb0ee7985b26d044319a60f916b00f469dc109.
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Downloads\eclipse-jee-mars-2-win32-x86_64\eclipse\DIGINode\surveillancetest\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\Survelince\surveillancetest\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="5"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="863" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Logintest" sheetId="22" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="LiveUnits" sheetId="25" r:id="rId4"/>
     <sheet name="AddNewUser" sheetId="26" r:id="rId5"/>
     <sheet name="Notifications" sheetId="27" r:id="rId6"/>
+    <sheet name="CreateNewClient" sheetId="28" r:id="rId7"/>
+    <sheet name="AddNewRoleTest" sheetId="29" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="222">
   <si>
     <t>TestID</t>
   </si>
@@ -76,12 +78,6 @@
     <t>LoginTest1</t>
   </si>
   <si>
-    <t>scott.abbott@liveviewtech.com</t>
-  </si>
-  <si>
-    <t>Royalfire1</t>
-  </si>
-  <si>
     <t>RevenuePerLiveUnitTest</t>
   </si>
   <si>
@@ -148,9 +144,6 @@
     <t>LVT Accounting</t>
   </si>
   <si>
-    <t>LVT Customer service" user</t>
-  </si>
-  <si>
     <t>LVT Infrastructure</t>
   </si>
   <si>
@@ -160,15 +153,9 @@
     <t>Camera Operator (Presets, PTZF)</t>
   </si>
   <si>
-    <t>Client administrator with Analytics</t>
-  </si>
-  <si>
     <t>RunMode</t>
   </si>
   <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -398,13 +385,331 @@
   </si>
   <si>
     <t>aatkinson@jacobsenconstruction.com</t>
+  </si>
+  <si>
+    <t>CreateNewClient</t>
+  </si>
+  <si>
+    <t>AccountRep</t>
+  </si>
+  <si>
+    <t>Timeout</t>
+  </si>
+  <si>
+    <t>LiveViewtes1</t>
+  </si>
+  <si>
+    <t>AUS ACT</t>
+  </si>
+  <si>
+    <t>IOS Dev</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>CreateNewClientWithAllFields</t>
+  </si>
+  <si>
+    <t>EmailDomain</t>
+  </si>
+  <si>
+    <t>ParentClient</t>
+  </si>
+  <si>
+    <t>BillableClient</t>
+  </si>
+  <si>
+    <t>SalesRep</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>SLA</t>
+  </si>
+  <si>
+    <t>SalesContact</t>
+  </si>
+  <si>
+    <t>SalesPhone</t>
+  </si>
+  <si>
+    <t>SalesMobile</t>
+  </si>
+  <si>
+    <t>SalesEmail</t>
+  </si>
+  <si>
+    <t>BillingContact</t>
+  </si>
+  <si>
+    <t>BillingPhone</t>
+  </si>
+  <si>
+    <t>BillingMobile</t>
+  </si>
+  <si>
+    <t>BillingEmail</t>
+  </si>
+  <si>
+    <t>TechnicalEmail</t>
+  </si>
+  <si>
+    <t>TechnicalContact</t>
+  </si>
+  <si>
+    <t>TechnicalPhone</t>
+  </si>
+  <si>
+    <t>TechnicalMobile</t>
+  </si>
+  <si>
+    <t>SecurityKey</t>
+  </si>
+  <si>
+    <t>MapCenterLatitude</t>
+  </si>
+  <si>
+    <t>MapCenterLongitude</t>
+  </si>
+  <si>
+    <t>MapZoomLevel</t>
+  </si>
+  <si>
+    <t>MapType</t>
+  </si>
+  <si>
+    <t>CameraNavigationMode</t>
+  </si>
+  <si>
+    <t>DefaultView</t>
+  </si>
+  <si>
+    <t>LogoImageName</t>
+  </si>
+  <si>
+    <t>VideoOverlayImage</t>
+  </si>
+  <si>
+    <t>AuthenticationEmailLinkDomain</t>
+  </si>
+  <si>
+    <t>ClientDomainRedirect</t>
+  </si>
+  <si>
+    <t>PublicVideoTimeout</t>
+  </si>
+  <si>
+    <t>PublicViewMode</t>
+  </si>
+  <si>
+    <t>OldFTPServer</t>
+  </si>
+  <si>
+    <t>WatermarkTextforImages</t>
+  </si>
+  <si>
+    <t>WelcomeEmailMessage</t>
+  </si>
+  <si>
+    <t>thisClientsUsers</t>
+  </si>
+  <si>
+    <t>OtherClientsUsers</t>
+  </si>
+  <si>
+    <t>StreamingServer</t>
+  </si>
+  <si>
+    <t>PatrolServer</t>
+  </si>
+  <si>
+    <t>DataExpiration</t>
+  </si>
+  <si>
+    <t>TermsOfServiceText</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>useD3CommandCenter</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>hyd</t>
+  </si>
+  <si>
+    <t>ind</t>
+  </si>
+  <si>
+    <t>mub</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>789</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Celsius</t>
+  </si>
+  <si>
+    <t>Liveview</t>
+  </si>
+  <si>
+    <t>AEDG</t>
+  </si>
+  <si>
+    <t>LVTA</t>
+  </si>
+  <si>
+    <t>www.lvt.com</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>abcde@gmail.com</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>Road Map</t>
+  </si>
+  <si>
+    <t>Plain Camera List</t>
+  </si>
+  <si>
+    <t>Camera Map</t>
+  </si>
+  <si>
+    <t>lvt</t>
+  </si>
+  <si>
+    <t>lvt1</t>
+  </si>
+  <si>
+    <t>http://abc@gmail.com</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Live Video</t>
+  </si>
+  <si>
+    <t>abcdefdg</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>hi live</t>
+  </si>
+  <si>
+    <t>Security Operator and Above</t>
+  </si>
+  <si>
+    <t>Client Admins and Above</t>
+  </si>
+  <si>
+    <t>UDOT</t>
+  </si>
+  <si>
+    <t>USW2A</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>hhhhh</t>
+  </si>
+  <si>
+    <t>klyn</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>test user title</t>
+  </si>
+  <si>
+    <t>Lvt international</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>AUS West</t>
+  </si>
+  <si>
+    <t>123-123-1234</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>AddNewRole</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TestRole</t>
+  </si>
+  <si>
+    <t>Test description</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Aaron Auer</t>
+  </si>
+  <si>
+    <t>aauer@nd.gov</t>
+  </si>
+  <si>
+    <t>1TestClient</t>
+  </si>
+  <si>
+    <t>Client Administrator with Analytics</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>UserEmaiIid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,6 +736,12 @@
       <color rgb="FF333333"/>
       <name val="Lucida Sans Unicode"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -472,7 +783,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -491,6 +802,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -814,14 +1128,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,13 +1166,16 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
+        <v>104</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -867,7 +1185,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +1199,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -898,7 +1216,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -909,34 +1227,38 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
@@ -944,16 +1266,16 @@
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -967,365 +1289,503 @@
         <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>18</v>
+        <v>220</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>19</v>
+        <v>221</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="J3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="L3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="6"/>
+      <c r="J5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
+        <v>104</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
+      <c r="L10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="L14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="J10" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="M17" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1336,7 +1796,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>0</v>
       </c>
@@ -1350,53 +1810,58 @@
         <v>11</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="G24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I24" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="M3" r:id="rId2" display="https://qa.liveviewtech.com/clients/view/1050/2"/>
+    <hyperlink ref="M12" r:id="rId3" display="https://qa.liveviewtech.com/clients/view/1050/2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1404,7 +1869,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1419,7 +1886,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1436,13 +1903,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1450,24 +1917,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1481,13 +1948,13 @@
         <v>11</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1495,16 +1962,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
@@ -1512,7 +1979,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1520,26 +1987,26 @@
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
         <v>73</v>
-      </c>
-      <c r="E13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="C13" r:id="rId2"/>
-    <hyperlink ref="C8" r:id="rId3"/>
+    <hyperlink ref="C13" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1550,7 +2017,7 @@
   <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,6 +2027,7 @@
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -1567,7 +2035,7 @@
   <sheetData>
     <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -1581,88 +2049,88 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="P2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="V2" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="P2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q2" s="8" t="s">
+      <c r="W2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="S2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="T2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>93</v>
-      </c>
       <c r="Z2" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AA2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="AD2" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -1670,50 +2138,123 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="N3" s="14">
+        <v>90001</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="U3" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J3" t="s">
-        <v>103</v>
-      </c>
-      <c r="W3" t="s">
-        <v>39</v>
-      </c>
-      <c r="X3" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>104</v>
-      </c>
+      <c r="Y3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC3" s="2"/>
       <c r="AD3" s="10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
       <c r="B4" s="11"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1730,8 +2271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,7 +2286,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1761,16 +2302,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1778,41 +2319,41 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" s="11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1820,9 +2361,932 @@
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="D9" r:id="rId2"/>
     <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4" display="https://qa.liveviewtech.com/users/view/5821"/>
+    <hyperlink ref="D3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CA7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="2"/>
+      <c r="BM1" s="2"/>
+      <c r="BN1" s="2"/>
+      <c r="BO1" s="2"/>
+      <c r="BP1" s="2"/>
+      <c r="BQ1" s="2"/>
+      <c r="BR1" s="2"/>
+      <c r="BS1" s="2"/>
+      <c r="BT1" s="2"/>
+      <c r="BU1" s="2"/>
+      <c r="BV1" s="2"/>
+      <c r="BW1" s="2"/>
+      <c r="BX1" s="2"/>
+      <c r="BY1" s="2"/>
+      <c r="BZ1" s="2"/>
+      <c r="CA1" s="2"/>
+    </row>
+    <row r="2" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+      <c r="BD2" s="2"/>
+      <c r="BE2" s="2"/>
+      <c r="BF2" s="2"/>
+      <c r="BG2" s="2"/>
+      <c r="BH2" s="2"/>
+      <c r="BI2" s="2"/>
+      <c r="BJ2" s="2"/>
+      <c r="BK2" s="2"/>
+      <c r="BL2" s="2"/>
+      <c r="BM2" s="2"/>
+      <c r="BN2" s="2"/>
+      <c r="BO2" s="2"/>
+      <c r="BP2" s="2"/>
+      <c r="BQ2" s="2"/>
+      <c r="BR2" s="2"/>
+      <c r="BS2" s="2"/>
+      <c r="BT2" s="2"/>
+      <c r="BU2" s="2"/>
+      <c r="BV2" s="2"/>
+      <c r="BW2" s="2"/>
+      <c r="BX2" s="2"/>
+      <c r="BY2" s="2"/>
+      <c r="BZ2" s="2"/>
+      <c r="CA2" s="2"/>
+    </row>
+    <row r="3" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2"/>
+      <c r="BE3" s="2"/>
+      <c r="BF3" s="2"/>
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2"/>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2"/>
+      <c r="BK3" s="2"/>
+      <c r="BL3" s="2"/>
+      <c r="BM3" s="2"/>
+      <c r="BN3" s="2"/>
+      <c r="BO3" s="2"/>
+      <c r="BP3" s="2"/>
+      <c r="BQ3" s="2"/>
+      <c r="BR3" s="2"/>
+      <c r="BS3" s="2"/>
+      <c r="BT3" s="2"/>
+      <c r="BU3" s="2"/>
+      <c r="BV3" s="2"/>
+      <c r="BW3" s="2"/>
+      <c r="BX3" s="2"/>
+      <c r="BY3" s="2"/>
+      <c r="BZ3" s="2"/>
+      <c r="CA3" s="2"/>
+    </row>
+    <row r="4" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="2"/>
+      <c r="BD4" s="2"/>
+      <c r="BE4" s="2"/>
+      <c r="BF4" s="2"/>
+      <c r="BG4" s="2"/>
+      <c r="BH4" s="2"/>
+      <c r="BI4" s="2"/>
+      <c r="BJ4" s="2"/>
+      <c r="BK4" s="2"/>
+      <c r="BL4" s="2"/>
+      <c r="BM4" s="2"/>
+      <c r="BN4" s="2"/>
+      <c r="BO4" s="2"/>
+      <c r="BP4" s="2"/>
+      <c r="BQ4" s="2"/>
+      <c r="BR4" s="2"/>
+      <c r="BS4" s="2"/>
+      <c r="BT4" s="2"/>
+      <c r="BU4" s="2"/>
+      <c r="BV4" s="2"/>
+      <c r="BW4" s="2"/>
+      <c r="BX4" s="2"/>
+      <c r="BY4" s="2"/>
+      <c r="BZ4" s="2"/>
+      <c r="CA4" s="2"/>
+    </row>
+    <row r="5" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="2"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="2"/>
+      <c r="BD5" s="2"/>
+      <c r="BE5" s="2"/>
+      <c r="BF5" s="2"/>
+      <c r="BG5" s="2"/>
+      <c r="BH5" s="2"/>
+      <c r="BI5" s="2"/>
+      <c r="BJ5" s="2"/>
+      <c r="BK5" s="2"/>
+      <c r="BL5" s="2"/>
+      <c r="BM5" s="2"/>
+      <c r="BN5" s="2"/>
+      <c r="BO5" s="2"/>
+      <c r="BP5" s="2"/>
+      <c r="BQ5" s="2"/>
+      <c r="BR5" s="2"/>
+      <c r="BS5" s="2"/>
+      <c r="BT5" s="2"/>
+      <c r="BU5" s="2"/>
+      <c r="BV5" s="2"/>
+      <c r="BW5" s="2"/>
+      <c r="BX5" s="2"/>
+      <c r="BY5" s="2"/>
+      <c r="BZ5" s="2"/>
+      <c r="CA5" s="2"/>
+    </row>
+    <row r="6" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA6" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB6" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG6" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH6" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI6" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ6" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK6" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL6" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN6" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AO6" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP6" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AR6" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AS6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT6" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AU6" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="AV6" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AX6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AY6" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AZ6" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="BA6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="BB6" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="BC6" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="BD6" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="BE6" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="BF6" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="BG6" s="7"/>
+      <c r="BH6" s="7"/>
+      <c r="BI6" s="7"/>
+      <c r="BJ6" s="7"/>
+      <c r="BK6" s="7"/>
+      <c r="BL6" s="7"/>
+      <c r="BM6" s="7"/>
+      <c r="BN6" s="7"/>
+      <c r="BO6" s="7"/>
+      <c r="BP6" s="7"/>
+      <c r="BQ6" s="7"/>
+      <c r="BR6" s="7"/>
+      <c r="BS6" s="7"/>
+      <c r="BT6" s="7"/>
+      <c r="BU6" s="7"/>
+      <c r="BV6" s="7"/>
+      <c r="BW6" s="7"/>
+      <c r="BX6" s="7"/>
+      <c r="BY6" s="7"/>
+      <c r="BZ6" s="7"/>
+      <c r="CA6" s="7"/>
+    </row>
+    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y7" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="AC7" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD7" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="AE7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF7" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="AG7" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="AH7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI7" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="AJ7" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="AK7" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="AL7" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="AM7" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="AN7" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="AO7" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="AP7" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="AQ7" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="AR7" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="AS7" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT7" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="AU7" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AV7" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AW7" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="AX7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AY7" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="AZ7" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="BA7" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="BB7" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="BC7" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="BD7" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="BE7" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="BF7" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="BG7" s="2"/>
+      <c r="BH7" s="2"/>
+      <c r="BI7" s="2"/>
+      <c r="BJ7" s="2"/>
+      <c r="BK7" s="2"/>
+      <c r="BL7" s="2"/>
+      <c r="BM7" s="2"/>
+      <c r="BN7" s="2"/>
+      <c r="BO7" s="2"/>
+      <c r="BP7" s="2"/>
+      <c r="BQ7" s="2"/>
+      <c r="BR7" s="2"/>
+      <c r="BS7" s="2"/>
+      <c r="BT7" s="2"/>
+      <c r="BU7" s="2"/>
+      <c r="BV7" s="2"/>
+      <c r="BW7" s="2"/>
+      <c r="BX7" s="2"/>
+      <c r="BY7" s="2"/>
+      <c r="BZ7" s="2"/>
+      <c r="CA7" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="H7" r:id="rId3"/>
+    <hyperlink ref="S7" r:id="rId4"/>
+    <hyperlink ref="Y7" r:id="rId5"/>
+    <hyperlink ref="AC7" r:id="rId6"/>
+    <hyperlink ref="AQ7" r:id="rId7"/>
+    <hyperlink ref="AD7" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the error message test cases.
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -9,22 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="10430" tabRatio="863" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="10430" tabRatio="863" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Logintest" sheetId="22" r:id="rId1"/>
     <sheet name="RevenuePerLiveUnitTest" sheetId="23" r:id="rId2"/>
     <sheet name="D3CommandCenterTest" sheetId="24" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="34" r:id="rId4"/>
-    <sheet name="BoxPageTest" sheetId="30" r:id="rId5"/>
-    <sheet name="ModemPageTest" sheetId="31" r:id="rId6"/>
-    <sheet name="HomePageTest" sheetId="32" r:id="rId7"/>
-    <sheet name="ViewProfilePageTest" sheetId="33" r:id="rId8"/>
-    <sheet name="LiveUnits" sheetId="25" r:id="rId9"/>
-    <sheet name="AddNewUser" sheetId="26" r:id="rId10"/>
-    <sheet name="Notifications" sheetId="27" r:id="rId11"/>
-    <sheet name="CreateNewClient" sheetId="28" r:id="rId12"/>
-    <sheet name="AddNewRoleTest" sheetId="29" r:id="rId13"/>
+    <sheet name="BoxPageTest" sheetId="30" r:id="rId4"/>
+    <sheet name="ModemPageTest" sheetId="31" r:id="rId5"/>
+    <sheet name="HomePageTest" sheetId="32" r:id="rId6"/>
+    <sheet name="ViewProfilePageTest" sheetId="33" r:id="rId7"/>
+    <sheet name="LiveUnits" sheetId="25" r:id="rId8"/>
+    <sheet name="AddNewUser" sheetId="26" r:id="rId9"/>
+    <sheet name="Notifications" sheetId="27" r:id="rId10"/>
+    <sheet name="CreateNewClient" sheetId="28" r:id="rId11"/>
+    <sheet name="AddNewRoleTest" sheetId="29" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="324">
   <si>
     <t>TestID</t>
   </si>
@@ -998,7 +997,16 @@
     <t>Camera Administrator (No Suspend/Archives)</t>
   </si>
   <si>
-    <t>NO</t>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>aauer@nd.gov</t>
+  </si>
+  <si>
+    <t>ResultsperPage</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -1483,260 +1491,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="2"/>
-    <col min="11" max="11" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD2" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE2" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="N3" s="13">
-        <v>90001</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="U3" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="V3" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE3" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="LVTTestAutomation@gmail.com"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1835,7 +1589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA7"/>
   <sheetViews>
@@ -2690,7 +2444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2826,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2895,7 +2649,7 @@
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>21</v>
@@ -2903,7 +2657,7 @@
       <c r="C3" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -2912,9 +2666,10 @@
       <c r="F3" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="5"/>
       <c r="L3" s="2" t="s">
         <v>37</v>
       </c>
@@ -2922,21 +2677,417 @@
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="L4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="L5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="L7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="L8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
@@ -2949,7 +3100,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>0</v>
       </c>
@@ -2978,7 +3129,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -3010,562 +3161,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D24" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M13" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>317</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
     <hyperlink ref="D4" r:id="rId2"/>
     <hyperlink ref="D5" r:id="rId3"/>
     <hyperlink ref="D6" r:id="rId4"/>
@@ -3579,12 +3174,14 @@
     <hyperlink ref="D14" r:id="rId12"/>
     <hyperlink ref="D15" r:id="rId13"/>
     <hyperlink ref="D16" r:id="rId14"/>
+    <hyperlink ref="D17" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -3661,7 +3258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU3"/>
   <sheetViews>
@@ -3971,7 +3568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -4024,7 +3621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG3"/>
   <sheetViews>
@@ -4241,7 +3838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -4381,4 +3978,271 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AE10" activeCellId="1" sqref="AG3 AE10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="2"/>
+    <col min="11" max="11" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="N3" s="13">
+        <v>90001</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF3" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="AG3" s="13" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="LVTTestAutomation@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="AF3" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
03-05-2024 OrangeHRM_Configuration Test Cases Completed
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91994\Desktop\RBG Project\RBGteamwork\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A26EC7-BE43-4ADE-BCB4-3D6E8EC4A9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87935321-40D7-4FAB-B43D-E1FEC45DFC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="922" firstSheet="15" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="582">
   <si>
     <t>TestID</t>
   </si>
@@ -1698,6 +1698,102 @@
   </si>
   <si>
     <t>rtgi.iug</t>
+  </si>
+  <si>
+    <t>UpdateOAuthName</t>
+  </si>
+  <si>
+    <t>UpdateReqiuredURI</t>
+  </si>
+  <si>
+    <t>madhu</t>
+  </si>
+  <si>
+    <t>tgsliafeh</t>
+  </si>
+  <si>
+    <t>HostName</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>publichost</t>
+  </si>
+  <si>
+    <t>UserAttribute</t>
+  </si>
+  <si>
+    <t>UserSearch</t>
+  </si>
+  <si>
+    <t>UserUnique</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Middlename</t>
+  </si>
+  <si>
+    <t>WorkemailBox</t>
+  </si>
+  <si>
+    <t>EmployIdBox</t>
+  </si>
+  <si>
+    <t>SyncBox</t>
+  </si>
+  <si>
+    <t>debt</t>
+  </si>
+  <si>
+    <t>ram</t>
+  </si>
+  <si>
+    <t>reddy</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>raj</t>
+  </si>
+  <si>
+    <t>rtb@gmail.comm</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>241</t>
+  </si>
+  <si>
+    <t>Distinguished</t>
+  </si>
+  <si>
+    <t>passwordname</t>
+  </si>
+  <si>
+    <t>BaseDistinguished</t>
+  </si>
+  <si>
+    <t>sekhar</t>
+  </si>
+  <si>
+    <t>Ramu</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>StatusBox</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>cmd</t>
   </si>
 </sst>
 </file>
@@ -4276,10 +4372,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12FA028C-D7DB-487B-896C-6B1A88662AEE}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:AK7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4303,14 +4399,27 @@
     <col min="18" max="18" width="17.77734375" customWidth="1"/>
     <col min="19" max="19" width="13.109375" customWidth="1"/>
     <col min="20" max="20" width="13.33203125" customWidth="1"/>
+    <col min="21" max="21" width="18" customWidth="1"/>
+    <col min="22" max="22" width="18.77734375" customWidth="1"/>
+    <col min="23" max="23" width="12.109375" customWidth="1"/>
+    <col min="24" max="24" width="13.5546875" customWidth="1"/>
+    <col min="25" max="25" width="19.77734375" customWidth="1"/>
+    <col min="26" max="26" width="17.88671875" customWidth="1"/>
+    <col min="27" max="27" width="20.21875" customWidth="1"/>
+    <col min="28" max="28" width="15.6640625" customWidth="1"/>
+    <col min="29" max="29" width="19.33203125" customWidth="1"/>
+    <col min="30" max="31" width="20.77734375" customWidth="1"/>
+    <col min="34" max="34" width="15.5546875" customWidth="1"/>
+    <col min="35" max="35" width="15.6640625" customWidth="1"/>
+    <col min="36" max="36" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>495</v>
       </c>
@@ -4363,7 +4472,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4416,12 +4525,12 @@
         <v>522</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>495</v>
       </c>
@@ -4482,8 +4591,59 @@
       <c r="T6" s="17" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U6" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="V6" s="17" t="s">
+        <v>551</v>
+      </c>
+      <c r="W6" s="17" t="s">
+        <v>554</v>
+      </c>
+      <c r="X6" s="17" t="s">
+        <v>555</v>
+      </c>
+      <c r="Y6" s="17" t="s">
+        <v>557</v>
+      </c>
+      <c r="Z6" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="AA6" s="17" t="s">
+        <v>559</v>
+      </c>
+      <c r="AB6" s="17" t="s">
+        <v>560</v>
+      </c>
+      <c r="AC6" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="AD6" s="17" t="s">
+        <v>562</v>
+      </c>
+      <c r="AE6" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="AF6" s="17" t="s">
+        <v>564</v>
+      </c>
+      <c r="AG6" s="17" t="s">
+        <v>568</v>
+      </c>
+      <c r="AH6" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="AI6" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="AJ6" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="AK6" s="17" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4543,6 +4703,57 @@
       </c>
       <c r="T7" t="s">
         <v>549</v>
+      </c>
+      <c r="U7" t="s">
+        <v>552</v>
+      </c>
+      <c r="V7" t="s">
+        <v>553</v>
+      </c>
+      <c r="W7" t="s">
+        <v>556</v>
+      </c>
+      <c r="X7" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="Y7" s="11" t="s">
+        <v>581</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>565</v>
+      </c>
+      <c r="AA7" s="11" t="s">
+        <v>572</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>566</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>567</v>
+      </c>
+      <c r="AD7" s="8" t="s">
+        <v>570</v>
+      </c>
+      <c r="AE7" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF7" s="11" t="s">
+        <v>578</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>569</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>576</v>
+      </c>
+      <c r="AI7">
+        <v>123456</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>577</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -4551,6 +4762,7 @@
     <hyperlink ref="H7" r:id="rId2" xr:uid="{5581FB1B-80E6-447F-A534-868B93631FAA}"/>
     <hyperlink ref="L7" r:id="rId3" xr:uid="{B0D163FC-5208-4FE9-A08B-98297F0FE4D2}"/>
     <hyperlink ref="P7" r:id="rId4" xr:uid="{5FA77D52-8F66-416F-AF2C-D8A5AF4BD0EA}"/>
+    <hyperlink ref="AD7" r:id="rId5" xr:uid="{8A6D3FE5-FB6C-4A10-8AD9-F75332338CD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>